<commit_message>
graded problem 2 assignment 1
</commit_message>
<xml_diff>
--- a/nivan/assignment1/grading.xlsx
+++ b/nivan/assignment1/grading.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
   <si>
     <t>Problem 1</t>
   </si>
@@ -159,6 +159,42 @@
   </si>
   <si>
     <t>3 (general idea, but code does not work)</t>
+  </si>
+  <si>
+    <t>10 (Fabios Solution?)</t>
+  </si>
+  <si>
+    <t>1 (the code did not work. The code is complex, I did not follow the code)</t>
+  </si>
+  <si>
+    <t>8 (general idea correct, but wrong check in the end)</t>
+  </si>
+  <si>
+    <t>3 (seems that you did not understand the concept of jolly)</t>
+  </si>
+  <si>
+    <t>9 (need to convert inputs to integers)</t>
+  </si>
+  <si>
+    <t>9 (any sequence with a single number is jolly!)</t>
+  </si>
+  <si>
+    <t>Obs</t>
+  </si>
+  <si>
+    <t>All your python files have merge conflicts, you should be careful when using more than one machine to work on the assignment.</t>
+  </si>
+  <si>
+    <t>7 (write idea, but logic is wrong! And any sequence with a single number is jolly!)</t>
+  </si>
+  <si>
+    <t>9 (the first element of the sequence is the sequence size and fails for sequences with only one element)</t>
+  </si>
+  <si>
+    <t>5 (seems that you did not understand well the concept of jolly, the code does not work in general)</t>
+  </si>
+  <si>
+    <t>9 (Missing indentation in the nested for's)</t>
   </si>
 </sst>
 </file>
@@ -174,12 +210,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -194,8 +236,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,19 +519,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="52.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="88.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="109.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -498,279 +543,385 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>37</v>
       </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
       <c r="D2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>15</v>
       </c>
       <c r="B14">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
       <c r="B15" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>17</v>
       </c>
       <c r="B16">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>18</v>
       </c>
       <c r="B17">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>19</v>
       </c>
       <c r="B18" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>20</v>
       </c>
       <c r="B19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>21</v>
       </c>
       <c r="B20">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>22</v>
       </c>
       <c r="B21" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>23</v>
       </c>
       <c r="B22" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>24</v>
       </c>
       <c r="B23">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>25</v>
       </c>
       <c r="B24">
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>26</v>
       </c>
       <c r="B25" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>27</v>
       </c>
       <c r="B26">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>28</v>
       </c>
       <c r="B27" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>29</v>
       </c>
       <c r="B28">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>30</v>
       </c>
       <c r="B29">
         <v>10</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>31</v>
       </c>
       <c r="B30">
         <v>10</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>32</v>
       </c>
       <c r="B31">
         <v>10</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>33</v>
       </c>
       <c r="B32" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>34</v>
       </c>
       <c r="B33">
         <v>10</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>35</v>
       </c>
       <c r="B34" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>36</v>
       </c>
       <c r="B35">
+        <v>10</v>
+      </c>
+      <c r="C35">
         <v>10</v>
       </c>
     </row>

</xml_diff>